<commit_message>
cambio carga masiva departamentos y sucursales
</commit_message>
<xml_diff>
--- a/configs/gestion-config/assets/excel-ejemplos/departamento.xlsx
+++ b/configs/gestion-config/assets/excel-ejemplos/departamento.xlsx
@@ -22,6 +22,9 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>Nombre departamento</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
   <si>
     <t>Departamento 1</t>
@@ -376,7 +379,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -399,7 +402,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -413,17 +418,26 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>123123</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>